<commit_message>
LTE code version and uploaded date
</commit_message>
<xml_diff>
--- a/Sensor Box Inventory /SensorBox_Component_Tracker.xlsx
+++ b/Sensor Box Inventory /SensorBox_Component_Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriishhate/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allensong/Documents/GitHub/CommonSENSES/Sensor Box Inventory /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC17B174-29CA-0D46-AB3D-557DA7CE24DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A9988F-FA96-1845-A0A4-5475C5BA19D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{9F8D9832-C5EF-1142-B4F9-7517213DD771}"/>
+    <workbookView xWindow="2600" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{9F8D9832-C5EF-1142-B4F9-7517213DD771}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Box Number</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>Cellular Module Name</t>
+  </si>
+  <si>
+    <t>Cellular Module Code Version</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>2_6</t>
   </si>
 </sst>
 </file>
@@ -424,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF163E4-59DB-9747-B16B-025799580D26}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,9 +444,10 @@
     <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,6 +456,17 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LTE ID and code uploaded date
LTE 01-55
</commit_message>
<xml_diff>
--- a/Sensor Box Inventory /SensorBox_Component_Tracker.xlsx
+++ b/Sensor Box Inventory /SensorBox_Component_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allensong/Documents/GitHub/CommonSENSES/Sensor Box Inventory /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A9988F-FA96-1845-A0A4-5475C5BA19D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E31DE3-2970-524B-B93B-8061DD03DD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{9F8D9832-C5EF-1142-B4F9-7517213DD771}"/>
+    <workbookView xWindow="7120" yWindow="1840" windowWidth="27640" windowHeight="16940" xr2:uid="{9F8D9832-C5EF-1142-B4F9-7517213DD771}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="116">
   <si>
     <t>Box Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Cellular Module Serial Number </t>
-  </si>
-  <si>
     <t>Cellular Module Name</t>
   </si>
   <si>
@@ -54,13 +51,346 @@
   </si>
   <si>
     <t>2_6</t>
+  </si>
+  <si>
+    <t>Cellular Module ID</t>
+  </si>
+  <si>
+    <t>e00fce688d4f56458911d5b9</t>
+  </si>
+  <si>
+    <t>e00fce6822227e153393a08f</t>
+  </si>
+  <si>
+    <t>e00fce68f3289e7bea49fe45</t>
+  </si>
+  <si>
+    <t>e00fce68773dd3b2c9843acb</t>
+  </si>
+  <si>
+    <t>e00fce684a184e44e3856757</t>
+  </si>
+  <si>
+    <t>e00fce68d97cb69773311ba4</t>
+  </si>
+  <si>
+    <t>e00fce68be7c34a7152a7849</t>
+  </si>
+  <si>
+    <t>e00fce682a3c3a77e8d5cef9</t>
+  </si>
+  <si>
+    <t>e00fce68cd4bb76b1b85dbe7</t>
+  </si>
+  <si>
+    <t>e00fce68d1acaa69840e983f</t>
+  </si>
+  <si>
+    <t>e00fce68a5b2cebf4cadf211</t>
+  </si>
+  <si>
+    <t>e00fce68cb9b730d1fdeb3ac</t>
+  </si>
+  <si>
+    <t>e00fce682af8b21e177ae3ac</t>
+  </si>
+  <si>
+    <t>e00fce682c905f7d061a9fc5</t>
+  </si>
+  <si>
+    <t>e00fce68fc48228349c6fa9b</t>
+  </si>
+  <si>
+    <t>e00fce6801e43b34ca838824</t>
+  </si>
+  <si>
+    <t>e00fce6895fb748aadf4347f</t>
+  </si>
+  <si>
+    <t>e00fce689ed0d46b5529b37a</t>
+  </si>
+  <si>
+    <t>e00fce6897349dcaadb7b012</t>
+  </si>
+  <si>
+    <t>e00fce6821c5d991c26b8f74</t>
+  </si>
+  <si>
+    <t>e00fce68fc0b02b755278fd4</t>
+  </si>
+  <si>
+    <t>e00fce688866629b967ad1c0</t>
+  </si>
+  <si>
+    <t>e00fce68f1266851ada437a3</t>
+  </si>
+  <si>
+    <t>e00fce6894d3f8daab014642</t>
+  </si>
+  <si>
+    <t>e00fce68e81a4b82eaf0e779</t>
+  </si>
+  <si>
+    <t>e00fce68e450b9311f8252c3</t>
+  </si>
+  <si>
+    <t>e00fce68f3bac6c04f7d7413</t>
+  </si>
+  <si>
+    <t>e00fce685cd2027fd2484c3e</t>
+  </si>
+  <si>
+    <t>e00fce68ba6e01f466e2b959</t>
+  </si>
+  <si>
+    <t>e00fce6880e944172c49cfd9</t>
+  </si>
+  <si>
+    <t>e00fce68682876ad21143888</t>
+  </si>
+  <si>
+    <t>e00fce689495e369536fcad7</t>
+  </si>
+  <si>
+    <t>e00fce681549aa118bc91a16</t>
+  </si>
+  <si>
+    <t>e00fce689901fcf4cd677c9a</t>
+  </si>
+  <si>
+    <t>e00fce687151b0efcb830758</t>
+  </si>
+  <si>
+    <t>e00fce68e21e8a5345f4e995</t>
+  </si>
+  <si>
+    <t>e00fce684e13ce8695c5858a</t>
+  </si>
+  <si>
+    <t>e00fce684c4c2b48532409de</t>
+  </si>
+  <si>
+    <t>e00fce689eb124b380614cab</t>
+  </si>
+  <si>
+    <t>e00fce687917e99dee0d69c9</t>
+  </si>
+  <si>
+    <t>e00fce689e04b8d421dbc3e6</t>
+  </si>
+  <si>
+    <t>e00fce68d3d422e69d735a96</t>
+  </si>
+  <si>
+    <t>e00fce680b2e2f19bcd46df8</t>
+  </si>
+  <si>
+    <t>e00fce6889265f915232cc01</t>
+  </si>
+  <si>
+    <t>e00fce684f68ac11f32133a3</t>
+  </si>
+  <si>
+    <t>e00fce68dde6d8dcf1a69540</t>
+  </si>
+  <si>
+    <t>e00fce682d33dce2e558f0ae</t>
+  </si>
+  <si>
+    <t>e00fce68c69df23b06ac4fcd</t>
+  </si>
+  <si>
+    <t>e00fce68cdc527709b827f96</t>
+  </si>
+  <si>
+    <t>e00fce68faedcae4a8bdde9e</t>
+  </si>
+  <si>
+    <t>e00fce68982f48df472d5123</t>
+  </si>
+  <si>
+    <t>e00fce6808b9077468904f69</t>
+  </si>
+  <si>
+    <t>e00fce6857b1ec7ab7e4545d</t>
+  </si>
+  <si>
+    <t>e00fce68430da86efd5d0e91</t>
+  </si>
+  <si>
+    <t>e00fce68c9ed1df3f8e2d2f9</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -73,6 +403,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -96,9 +432,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,17 +772,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF163E4-59DB-9747-B16B-025799580D26}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -452,24 +791,790 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D52" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="2">
+        <v>45793</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>